<commit_message>
printed hex value for each building location
</commit_message>
<xml_diff>
--- a/GameBoards.xlsx
+++ b/GameBoards.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethhsu/Google Drive/Hsu Family/Kenneth Hsu/Projects/Colonizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AD8DB2-2EA9-6C42-98D6-C9C972BFE5DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8586F57-664A-DE48-9568-B9430E3E1C68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3600" yWindow="2600" windowWidth="28040" windowHeight="17440" xr2:uid="{ECD0B745-F889-C448-A747-C36281352244}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="35">
   <si>
     <t>Game</t>
   </si>
@@ -487,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B0F4AA2-A4EF-0047-9E07-AE4E15987399}">
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -762,6 +762,184 @@
         <v>31</v>
       </c>
     </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" t="s">
+        <v>33</v>
+      </c>
+      <c r="U4" t="s">
+        <v>31</v>
+      </c>
+      <c r="V4" t="s">
+        <v>31</v>
+      </c>
+      <c r="W4" t="s">
+        <v>29</v>
+      </c>
+      <c r="X4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U5" t="s">
+        <v>33</v>
+      </c>
+      <c r="V5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
dice assignment direction done, but offset is not
</commit_message>
<xml_diff>
--- a/GameBoards.xlsx
+++ b/GameBoards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethhsu/Google Drive/Hsu Family/Kenneth Hsu/Projects/Colonizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8586F57-664A-DE48-9568-B9430E3E1C68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8C99CB-B891-7448-A66A-6A4E42ECDD9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="2600" windowWidth="28040" windowHeight="17440" xr2:uid="{ECD0B745-F889-C448-A747-C36281352244}"/>
+    <workbookView xWindow="0" yWindow="1040" windowWidth="33600" windowHeight="20500" xr2:uid="{ECD0B745-F889-C448-A747-C36281352244}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="37">
   <si>
     <t>Game</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>sheep</t>
+  </si>
+  <si>
+    <t>﻿diceSetupHexOffset</t>
+  </si>
+  <si>
+    <t>﻿diceSetupClockwise</t>
   </si>
 </sst>
 </file>
@@ -487,15 +493,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B0F4AA2-A4EF-0047-9E07-AE4E15987399}">
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AC5" sqref="AC5"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="30" max="30" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -583,8 +593,14 @@
       <c r="AC1" t="s">
         <v>28</v>
       </c>
+      <c r="AD1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -672,8 +688,14 @@
       <c r="AC2" t="s">
         <v>29</v>
       </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -761,8 +783,14 @@
       <c r="AC3" t="s">
         <v>31</v>
       </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -850,8 +878,14 @@
       <c r="AC4" t="s">
         <v>34</v>
       </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -938,6 +972,202 @@
       </c>
       <c r="AC5" t="s">
         <v>32</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>29</v>
+      </c>
+      <c r="R6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S6" t="s">
+        <v>30</v>
+      </c>
+      <c r="T6" t="s">
+        <v>31</v>
+      </c>
+      <c r="U6" t="s">
+        <v>32</v>
+      </c>
+      <c r="V6" t="s">
+        <v>29</v>
+      </c>
+      <c r="W6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>31</v>
+      </c>
+      <c r="R7" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7" t="s">
+        <v>29</v>
+      </c>
+      <c r="T7" t="s">
+        <v>30</v>
+      </c>
+      <c r="U7" t="s">
+        <v>32</v>
+      </c>
+      <c r="V7" t="s">
+        <v>33</v>
+      </c>
+      <c r="W7" t="s">
+        <v>34</v>
+      </c>
+      <c r="X7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD7">
+        <v>-2</v>
+      </c>
+      <c r="AE7" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dice assignemnt with offset is done
</commit_message>
<xml_diff>
--- a/GameBoards.xlsx
+++ b/GameBoards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethhsu/Google Drive/Hsu Family/Kenneth Hsu/Projects/Colonizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8C99CB-B891-7448-A66A-6A4E42ECDD9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB609C57-C289-0142-9486-338F23141FDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1040" windowWidth="33600" windowHeight="20500" xr2:uid="{ECD0B745-F889-C448-A747-C36281352244}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{ECD0B745-F889-C448-A747-C36281352244}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -496,7 +496,7 @@
   <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AD7" sqref="AD7"/>
+      <selection activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1072,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="AE6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
@@ -1164,7 +1164,7 @@
         <v>30</v>
       </c>
       <c r="AD7">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="AE7" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Able to detect which building is clicked
</commit_message>
<xml_diff>
--- a/GameBoards.xlsx
+++ b/GameBoards.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethhsu/Google Drive/Hsu Family/Kenneth Hsu/Projects/Colonizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5085A69C-EAD9-D04C-A9C2-3D902C5C2FBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35E7B1A-49DF-1547-9CD8-82347C12F808}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{ECD0B745-F889-C448-A747-C36281352244}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,63 +30,6 @@
     <t>Game</t>
   </si>
   <si>
-    <t>Tile 1</t>
-  </si>
-  <si>
-    <t>Tile 2</t>
-  </si>
-  <si>
-    <t>Tile 3</t>
-  </si>
-  <si>
-    <t>Tile 4</t>
-  </si>
-  <si>
-    <t>Tile 5</t>
-  </si>
-  <si>
-    <t>Tile 6</t>
-  </si>
-  <si>
-    <t>Tile 7</t>
-  </si>
-  <si>
-    <t>Tile 8</t>
-  </si>
-  <si>
-    <t>Tile 9</t>
-  </si>
-  <si>
-    <t>Tile 10</t>
-  </si>
-  <si>
-    <t>Tile 11</t>
-  </si>
-  <si>
-    <t>Tile 12</t>
-  </si>
-  <si>
-    <t>Tile 13</t>
-  </si>
-  <si>
-    <t>Tile 14</t>
-  </si>
-  <si>
-    <t>Tile 15</t>
-  </si>
-  <si>
-    <t>Tile 16</t>
-  </si>
-  <si>
-    <t>Tile 17</t>
-  </si>
-  <si>
-    <t>Tile 18</t>
-  </si>
-  <si>
-    <t>Tile 19</t>
-  </si>
-  <si>
     <t>Port 1</t>
   </si>
   <si>
@@ -132,10 +75,67 @@
     <t>sheep</t>
   </si>
   <si>
-    <t>﻿diceSetupHexOffset</t>
-  </si>
-  <si>
-    <t>﻿diceSetupClockwise</t>
+    <t>Row 1 Tile 1</t>
+  </si>
+  <si>
+    <t>Row 1 Tile 2</t>
+  </si>
+  <si>
+    <t>Row 1 Tile 3</t>
+  </si>
+  <si>
+    <t>Row 2 Tile 1</t>
+  </si>
+  <si>
+    <t>Row 2 Tile 2</t>
+  </si>
+  <si>
+    <t>Row 2 Tile 3</t>
+  </si>
+  <si>
+    <t>Row 2 Tile 4</t>
+  </si>
+  <si>
+    <t>Row 3 Tile 1</t>
+  </si>
+  <si>
+    <t>Row 3 Tile 2</t>
+  </si>
+  <si>
+    <t>Row 3 Tile 3</t>
+  </si>
+  <si>
+    <t>Row 3 Tile 4</t>
+  </si>
+  <si>
+    <t>Row 3 Tile 5</t>
+  </si>
+  <si>
+    <t>Row 4 Tile 1</t>
+  </si>
+  <si>
+    <t>Row 4 Tile 2</t>
+  </si>
+  <si>
+    <t>Row 4 Tile 3</t>
+  </si>
+  <si>
+    <t>Row 4 Tile 4</t>
+  </si>
+  <si>
+    <t>Row 5 Tile 1</t>
+  </si>
+  <si>
+    <t>Row 5 Tile 2</t>
+  </si>
+  <si>
+    <t>Row 5 Tile 3</t>
+  </si>
+  <si>
+    <t>"5" Starting Location Offset</t>
+  </si>
+  <si>
+    <t>ClockwiseDiceSetup</t>
   </si>
 </sst>
 </file>
@@ -177,8 +177,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,103 +498,106 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B0F4AA2-A4EF-0047-9E07-AE4E15987399}">
   <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AE8" sqref="AE8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="30" max="30" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="29" width="11" customWidth="1"/>
+    <col min="30" max="30" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="V1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="W1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="X1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="Y1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="Z1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="AA1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="AB1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="AC1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
       </c>
       <c r="AD1" t="s">
         <v>35</v>
@@ -601,92 +607,92 @@
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="M2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="N2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="O2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="P2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="Q2" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="R2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="S2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="T2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="U2" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="V2" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="W2" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="X2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="Y2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="Z2" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="AA2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="AB2" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="AC2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="AD2">
         <v>0</v>
@@ -696,92 +702,92 @@
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="M3" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="N3" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="O3" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="P3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="Q3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="R3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="S3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="T3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="U3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="V3" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="W3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="X3" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="Y3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="Z3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="AA3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="AB3" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="AC3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="AD3">
         <v>0</v>
@@ -791,92 +797,92 @@
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="L4" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="M4" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="N4" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="P4" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="Q4" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="R4" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="S4" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="T4" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="U4" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="V4" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="W4" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="X4" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="Y4" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="Z4" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="AA4" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="AB4" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="AC4" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="AD4">
         <v>0</v>
@@ -886,92 +892,92 @@
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="M5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="N5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="O5" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="P5" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="Q5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="R5" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="S5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="T5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="U5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="V5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="W5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="X5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="Y5" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="Z5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="AA5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="AB5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="AC5" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="AD5">
         <v>0</v>
@@ -981,92 +987,92 @@
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="K6" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="L6" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="M6" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="N6" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="O6" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="P6" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="Q6" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="R6" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="S6" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="T6" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="U6" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="V6" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="W6" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="X6" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="Y6" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="Z6" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="AA6" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="AB6" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="AC6" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="AD6">
         <v>0</v>
@@ -1076,92 +1082,92 @@
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="J7" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="K7" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="M7" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="N7" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="O7" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="P7" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="Q7" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="R7" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="S7" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="T7" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="U7" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="V7" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="W7" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="X7" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="Y7" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="Z7" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="AA7" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="AB7" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="AC7" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="AD7">
         <v>2</v>

</xml_diff>